<commit_message>
feat: load isoautocorr data
resolves #954
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/isoautocorr/test-isoautocorr-study/test-isoautocorr-negative-cor.xlsx
+++ b/DataRepo/data/tests/isoautocorr/test-isoautocorr-study/test-isoautocorr-negative-cor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" state="visible" r:id="rId2"/>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">C12 PARENT</t>
   </si>
   <si>
-    <t xml:space="preserve">L-Serine</t>
+    <t xml:space="preserve">serine</t>
   </si>
   <si>
     <t xml:space="preserve">C3H7NO3</t>
@@ -227,8 +227,8 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="B2 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -339,10 +339,10 @@
       <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -394,10 +394,10 @@
       <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -449,10 +449,10 @@
       <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -504,10 +504,10 @@
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -559,10 +559,10 @@
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -614,10 +614,10 @@
       <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -669,10 +669,10 @@
       <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -724,10 +724,10 @@
       <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="B2 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1217,10 +1217,10 @@
       <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1272,10 +1272,10 @@
       <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -1327,10 +1327,10 @@
       <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1382,10 +1382,10 @@
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1437,10 +1437,10 @@
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1492,10 +1492,10 @@
       <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -1547,10 +1547,10 @@
       <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1602,10 +1602,10 @@
       <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1984,7 +1984,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="B2 K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2095,10 +2095,10 @@
       <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -2150,10 +2150,10 @@
       <c r="I3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -2205,10 +2205,10 @@
       <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -2260,10 +2260,10 @@
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -2315,10 +2315,10 @@
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -2370,10 +2370,10 @@
       <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -2425,10 +2425,10 @@
       <c r="I8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -2480,10 +2480,10 @@
       <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -2861,8 +2861,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2904,7 +2904,7 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">

</xml_diff>